<commit_message>
Update automatico via Actualizar 11-10-2020 17-11-10
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="103" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{67BD469F-D135-43C0-864C-751C180BD187}"/>
+  <xr:revisionPtr revIDLastSave="104" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6CB89255-BF3F-4186-B868-0EA2A171A6F2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Dia</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>Banco Central de Chile - Indicadores diarios - Precio del Cobre, dólares por libra (Dólar) - Años 2019 - 2020</t>
-  </si>
-  <si>
-    <t>p</t>
   </si>
 </sst>
 </file>
@@ -1172,13 +1169,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2937"/>
+  <dimension ref="A1:C2938"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B2926" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A2935" sqref="A2935:B2937"/>
+      <selection pane="bottomRight" activeCell="B2938" sqref="B2938"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23175,8 +23172,8 @@
       </c>
     </row>
     <row r="2935" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2935" s="92" t="s">
-        <v>3</v>
+      <c r="A2935" s="92">
+        <v>44142</v>
       </c>
       <c r="B2935" s="93"/>
     </row>
@@ -23192,6 +23189,14 @@
       </c>
       <c r="B2937" s="93">
         <v>3.1038999999999999</v>
+      </c>
+    </row>
+    <row r="2938" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2938" s="92">
+        <v>44145</v>
+      </c>
+      <c r="B2938" s="93">
+        <v>3.1457000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-11-2020 15-49-17
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6CB89255-BF3F-4186-B868-0EA2A171A6F2}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A4D909DE-E667-4375-B30C-494C627389A6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -546,6 +546,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1169,13 +1175,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2938"/>
+  <dimension ref="A1:C2939"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B2926" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B2938" sqref="B2938"/>
+      <selection pane="bottomRight" activeCell="B2939" sqref="B2939"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23199,6 +23205,14 @@
         <v>3.1457000000000002</v>
       </c>
     </row>
+    <row r="2939" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2939" s="94">
+        <v>44146</v>
+      </c>
+      <c r="B2939" s="95">
+        <v>3.1313</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2731" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-13-2020 17-15-09
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="108" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0ED1B662-06FE-4648-A4CC-FD93CA9F4DA6}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D5B4FCEB-7961-4D88-9E89-E493F4838532}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -546,6 +546,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1181,13 +1187,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2940"/>
+  <dimension ref="A1:C2941"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B2931" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B2937" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B2940" sqref="B2940"/>
+      <selection pane="bottomRight" activeCell="B2941" sqref="B2941"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23227,6 +23233,14 @@
         <v>3.1358000000000001</v>
       </c>
     </row>
+    <row r="2941" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2941" s="98">
+        <v>44148</v>
+      </c>
+      <c r="B2941" s="99">
+        <v>3.1143999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2731" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-14-2020 17-06-29
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D5B4FCEB-7961-4D88-9E89-E493F4838532}"/>
+  <xr:revisionPtr revIDLastSave="110" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5BE0A2C2-5E75-4A4A-AA4C-B23CBAD451D0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1187,13 +1187,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2941"/>
+  <dimension ref="A1:C2944"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B2937" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B2941" sqref="B2941"/>
+      <selection pane="bottomRight" activeCell="A2944" sqref="A2944"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23241,6 +23241,26 @@
         <v>3.1143999999999998</v>
       </c>
     </row>
+    <row r="2942" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2942" s="98">
+        <v>44149</v>
+      </c>
+      <c r="B2942" s="99"/>
+    </row>
+    <row r="2943" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2943" s="98">
+        <v>44150</v>
+      </c>
+      <c r="B2943" s="99"/>
+    </row>
+    <row r="2944" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2944" s="98">
+        <v>44151</v>
+      </c>
+      <c r="B2944" s="99">
+        <v>3.137</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2731" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-18-2020 17-10-25
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="110" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5BE0A2C2-5E75-4A4A-AA4C-B23CBAD451D0}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B1C98160-3E85-45B3-B1E7-D7FCB9BB83B6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -546,6 +546,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1187,13 +1193,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2944"/>
+  <dimension ref="A1:C2946"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B2937" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A2944" sqref="A2944"/>
+      <selection pane="bottomRight" activeCell="B2946" sqref="B2946"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23261,6 +23267,22 @@
         <v>3.137</v>
       </c>
     </row>
+    <row r="2945" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2945" s="100">
+        <v>44152</v>
+      </c>
+      <c r="B2945" s="101">
+        <v>3.1598999999999999</v>
+      </c>
+    </row>
+    <row r="2946" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2946" s="100">
+        <v>44153</v>
+      </c>
+      <c r="B2946" s="101">
+        <v>3.2172999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2731" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-19-2020 17-13-02
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B1C98160-3E85-45B3-B1E7-D7FCB9BB83B6}"/>
+  <xr:revisionPtr revIDLastSave="112" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{060F3AE5-7467-4B9C-82C0-65A9EA865786}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -546,6 +546,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1193,13 +1199,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2946"/>
+  <dimension ref="A1:C2947"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B2937" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B2946" sqref="B2946"/>
+      <selection pane="bottomRight" activeCell="B2947" sqref="B2947"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23283,6 +23289,14 @@
         <v>3.2172999999999998</v>
       </c>
     </row>
+    <row r="2947" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2947" s="102">
+        <v>44154</v>
+      </c>
+      <c r="B2947" s="103">
+        <v>3.1964999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2731" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-20-2020 17-09-44
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="112" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{060F3AE5-7467-4B9C-82C0-65A9EA865786}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C90DFD74-8F1E-4EAA-B660-EEC7868C2EAF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -546,6 +546,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1199,13 +1205,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2947"/>
+  <dimension ref="A1:C2948"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B2937" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B2947" sqref="B2947"/>
+      <selection pane="bottomRight" activeCell="B2948" sqref="B2948"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23297,6 +23303,14 @@
         <v>3.1964999999999999</v>
       </c>
     </row>
+    <row r="2948" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2948" s="104">
+        <v>44155</v>
+      </c>
+      <c r="B2948" s="105">
+        <v>3.2067000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2731" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-21-2020 17-08-36
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C90DFD74-8F1E-4EAA-B660-EEC7868C2EAF}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4A837E76-9098-4E94-A2D5-81E6CA485361}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -546,6 +546,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1205,13 +1211,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2948"/>
+  <dimension ref="A1:C2951"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B2937" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B2948" sqref="B2948"/>
+      <selection pane="bottomRight" activeCell="A2952" sqref="A2952"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23311,6 +23317,26 @@
         <v>3.2067000000000001</v>
       </c>
     </row>
+    <row r="2949" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2949" s="106">
+        <v>44156</v>
+      </c>
+      <c r="B2949" s="107"/>
+    </row>
+    <row r="2950" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2950" s="106">
+        <v>44157</v>
+      </c>
+      <c r="B2950" s="107"/>
+    </row>
+    <row r="2951" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2951" s="106">
+        <v>44158</v>
+      </c>
+      <c r="B2951" s="107">
+        <v>3.2098</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2731" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-24-2020 17-09-14
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4A837E76-9098-4E94-A2D5-81E6CA485361}"/>
+  <xr:revisionPtr revIDLastSave="116" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0BCC1C3C-884F-4F36-A1DE-C5E3FE0DD580}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -832,6 +832,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1211,13 +1217,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2951"/>
+  <dimension ref="A1:C2952"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B2937" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A2952" sqref="A2952"/>
+      <selection pane="bottomRight" activeCell="B2954" sqref="B2954"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23337,6 +23343,14 @@
         <v>3.2098</v>
       </c>
     </row>
+    <row r="2952" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2952" s="109">
+        <v>44159</v>
+      </c>
+      <c r="B2952" s="108">
+        <v>3.2942</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2731" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-25-2020 17-13-32
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="116" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0BCC1C3C-884F-4F36-A1DE-C5E3FE0DD580}"/>
+  <xr:revisionPtr revIDLastSave="117" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F4FC00AA-ADEE-45A8-BE4F-48F8C295D4C1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1217,13 +1217,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2952"/>
+  <dimension ref="A1:C2953"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B2937" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B2951" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B2954" sqref="B2954"/>
+      <selection pane="bottomRight" activeCell="B2953" sqref="B2953"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23351,6 +23351,14 @@
         <v>3.2942</v>
       </c>
     </row>
+    <row r="2953" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2953" s="109">
+        <v>44160</v>
+      </c>
+      <c r="B2953" s="108">
+        <v>3.2486999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2731" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-26-2020 17-07-32
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="117" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F4FC00AA-ADEE-45A8-BE4F-48F8C295D4C1}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0A2FA631-14B4-47EA-B9DF-5326CE9E7921}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -838,6 +838,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1217,13 +1223,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2953"/>
+  <dimension ref="A1:C2954"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B2951" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B2953" sqref="B2953"/>
+      <selection pane="bottomRight" activeCell="A2955" sqref="A2955"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23359,6 +23365,14 @@
         <v>3.2486999999999999</v>
       </c>
     </row>
+    <row r="2954" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2954" s="110">
+        <v>44161</v>
+      </c>
+      <c r="B2954" s="111">
+        <v>3.3018000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2731" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-27-2020 17-06-11
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0A2FA631-14B4-47EA-B9DF-5326CE9E7921}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AF3B70B0-1DD0-432E-B625-F1861BC029D6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -838,6 +838,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1223,13 +1229,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2954"/>
+  <dimension ref="A1:C2955"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B2951" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A2955" sqref="A2955"/>
+      <selection pane="bottomRight" activeCell="A2958" sqref="A2958"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23373,6 +23379,14 @@
         <v>3.3018000000000001</v>
       </c>
     </row>
+    <row r="2955" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2955" s="112">
+        <v>44162</v>
+      </c>
+      <c r="B2955" s="113">
+        <v>3.3037000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2731" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-28-2020 17-12-50
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="119" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AF3B70B0-1DD0-432E-B625-F1861BC029D6}"/>
+  <xr:revisionPtr revIDLastSave="120" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{61D7D701-61D4-43C4-A948-44D02C177424}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -838,6 +838,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1229,7 +1235,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2955"/>
+  <dimension ref="A1:C2958"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B2951" activePane="bottomRight" state="frozen"/>
@@ -23387,6 +23393,26 @@
         <v>3.3037000000000001</v>
       </c>
     </row>
+    <row r="2956" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2956" s="114">
+        <v>44163</v>
+      </c>
+      <c r="B2956" s="115"/>
+    </row>
+    <row r="2957" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2957" s="114">
+        <v>44164</v>
+      </c>
+      <c r="B2957" s="115"/>
+    </row>
+    <row r="2958" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2958" s="114">
+        <v>44165</v>
+      </c>
+      <c r="B2958" s="115">
+        <v>3.3506999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2731" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-01-2020 17-05-48
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="120" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{61D7D701-61D4-43C4-A948-44D02C177424}"/>
+  <xr:revisionPtr revIDLastSave="124" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2E3F0B38-5776-4951-A102-4A52C10ADB69}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -838,6 +838,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1235,13 +1241,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2958"/>
+  <dimension ref="A1:C2959"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B2951" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A2958" sqref="A2958"/>
+      <selection pane="bottomRight" activeCell="B2959" sqref="B2959"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23413,6 +23419,14 @@
         <v>3.3506999999999998</v>
       </c>
     </row>
+    <row r="2959" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2959" s="116">
+        <v>44166</v>
+      </c>
+      <c r="B2959" s="117">
+        <v>3.3963000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2731" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-03-2020 17-05-57
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="124" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2E3F0B38-5776-4951-A102-4A52C10ADB69}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C1E175DF-1565-4787-9A67-115FC9B5D2AC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -838,6 +838,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1241,13 +1247,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2959"/>
+  <dimension ref="A1:C2961"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B2951" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B2959" sqref="B2959"/>
+      <selection pane="bottomRight" activeCell="B2961" sqref="B2961"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23427,6 +23433,22 @@
         <v>3.3963000000000001</v>
       </c>
     </row>
+    <row r="2960" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2960" s="118">
+        <v>44167</v>
+      </c>
+      <c r="B2960" s="119">
+        <v>3.4333999999999998</v>
+      </c>
+    </row>
+    <row r="2961" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2961" s="118">
+        <v>44168</v>
+      </c>
+      <c r="B2961" s="119">
+        <v>3.4872999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2731" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-04-2020 19-14-04
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C1E175DF-1565-4787-9A67-115FC9B5D2AC}"/>
+  <xr:revisionPtr revIDLastSave="126" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{91BBB3E0-BC9C-45A2-8F64-8E06855E257C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -838,6 +838,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1247,13 +1253,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2961"/>
+  <dimension ref="A1:C2962"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B2951" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B2954" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B2961" sqref="B2961"/>
+      <selection pane="bottomRight" activeCell="A2963" sqref="A2963"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23449,6 +23455,14 @@
         <v>3.4872999999999998</v>
       </c>
     </row>
+    <row r="2962" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2962" s="120">
+        <v>44169</v>
+      </c>
+      <c r="B2962" s="121">
+        <v>3.4775</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2731" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-10-2020 17-10-55
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="131" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{617B0909-9C6C-4A11-8FD0-E1454A571AF4}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D985DB4C-320B-4021-A291-B43CFB060187}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -880,6 +880,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1259,13 +1265,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2967"/>
+  <dimension ref="A1:C2968"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B2960" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A2967" sqref="A2967"/>
+      <selection pane="bottomRight" activeCell="B2968" sqref="B2968"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23503,6 +23509,14 @@
         <v>3.5156999999999998</v>
       </c>
     </row>
+    <row r="2968" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2968" s="125">
+        <v>44175</v>
+      </c>
+      <c r="B2968" s="124">
+        <v>3.4832000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2731" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-10-2020 20-50-38
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="133" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D985DB4C-320B-4021-A291-B43CFB060187}"/>
+  <xr:revisionPtr revIDLastSave="137" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FBE18171-D138-4D35-AB0A-1FA0FE347A5B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -880,6 +880,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1265,13 +1271,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2968"/>
+  <dimension ref="A1:C2969"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B2960" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B2962" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B2968" sqref="B2968"/>
+      <selection pane="bottomRight" activeCell="A2969" sqref="A2969"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23517,6 +23523,14 @@
         <v>3.4832000000000001</v>
       </c>
     </row>
+    <row r="2969" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2969" s="127">
+        <v>44176</v>
+      </c>
+      <c r="B2969" s="126">
+        <v>3.4952000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2731" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-12-2020 17-07-52
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="137" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FBE18171-D138-4D35-AB0A-1FA0FE347A5B}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CD158C9D-77E2-4621-953D-2CCC9B223F63}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -892,6 +892,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1271,13 +1277,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2969"/>
+  <dimension ref="A1:C2972"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B2962" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A2969" sqref="A2969"/>
+      <selection pane="bottomRight" activeCell="A2972" sqref="A2972"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23531,6 +23537,26 @@
         <v>3.4952000000000001</v>
       </c>
     </row>
+    <row r="2970" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2970" s="128">
+        <v>44177</v>
+      </c>
+      <c r="B2970" s="129"/>
+    </row>
+    <row r="2971" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2971" s="128">
+        <v>44178</v>
+      </c>
+      <c r="B2971" s="129"/>
+    </row>
+    <row r="2972" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2972" s="128">
+        <v>44179</v>
+      </c>
+      <c r="B2972" s="129">
+        <v>3.5655999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2731" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-15-2020 17-13-35
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="138" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CD158C9D-77E2-4621-953D-2CCC9B223F63}"/>
+  <xr:revisionPtr revIDLastSave="139" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5B3578B6-B6B2-4B19-8DE3-DC890A053933}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -892,6 +892,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1277,13 +1283,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2972"/>
+  <dimension ref="A1:C2973"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B2962" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B2968" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A2972" sqref="A2972"/>
+      <selection pane="bottomRight" activeCell="A2973" sqref="A2973"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23557,6 +23563,14 @@
         <v>3.5655999999999999</v>
       </c>
     </row>
+    <row r="2973" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2973" s="130">
+        <v>44180</v>
+      </c>
+      <c r="B2973" s="131">
+        <v>3.5175999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2731" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-16-2020 17-05-18
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="139" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5B3578B6-B6B2-4B19-8DE3-DC890A053933}"/>
+  <xr:revisionPtr revIDLastSave="140" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4F8C6E58-25CA-47EA-9560-B21A4EFDA4A8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -892,6 +892,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1283,13 +1289,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2973"/>
+  <dimension ref="A1:C2974"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B2968" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A2973" sqref="A2973"/>
+      <selection pane="bottomRight" activeCell="A2975" sqref="A2975"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23571,6 +23577,14 @@
         <v>3.5175999999999998</v>
       </c>
     </row>
+    <row r="2974" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2974" s="132">
+        <v>44181</v>
+      </c>
+      <c r="B2974" s="133">
+        <v>3.5059</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2731" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-17-2020 17-07-32
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="140" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4F8C6E58-25CA-47EA-9560-B21A4EFDA4A8}"/>
+  <xr:revisionPtr revIDLastSave="141" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5E95D582-C188-4E04-82AB-D685550A8780}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -892,6 +892,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1289,13 +1295,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2974"/>
+  <dimension ref="A1:C2975"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B2968" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A2975" sqref="A2975"/>
+      <selection pane="bottomRight" activeCell="A2976" sqref="A2976"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23585,6 +23591,14 @@
         <v>3.5059</v>
       </c>
     </row>
+    <row r="2975" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2975" s="134">
+        <v>44182</v>
+      </c>
+      <c r="B2975" s="135">
+        <v>3.5203000000000002</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2731" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-18-2020 17-12-28
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="141" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5E95D582-C188-4E04-82AB-D685550A8780}"/>
+  <xr:revisionPtr revIDLastSave="142" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{032E74D9-C235-4FDF-8C01-2843CF9CE2C8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -892,6 +892,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1295,13 +1301,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2975"/>
+  <dimension ref="A1:C2976"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B2968" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A2976" sqref="A2976"/>
+      <selection pane="bottomRight" activeCell="B2976" sqref="B2976"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23599,6 +23605,14 @@
         <v>3.5203000000000002</v>
       </c>
     </row>
+    <row r="2976" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2976" s="136">
+        <v>44183</v>
+      </c>
+      <c r="B2976" s="137">
+        <v>3.5442</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2731" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-19-2020 17-05-58
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="142" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{032E74D9-C235-4FDF-8C01-2843CF9CE2C8}"/>
+  <xr:revisionPtr revIDLastSave="143" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E563F784-413D-493B-A73B-C6CA1A386172}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1301,13 +1301,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2976"/>
+  <dimension ref="A1:C2979"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B2968" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B2976" sqref="B2976"/>
+      <selection pane="bottomRight" activeCell="A2979" sqref="A2979"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23613,6 +23613,26 @@
         <v>3.5442</v>
       </c>
     </row>
+    <row r="2977" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2977" s="136">
+        <v>44184</v>
+      </c>
+      <c r="B2977" s="137"/>
+    </row>
+    <row r="2978" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2978" s="136">
+        <v>44185</v>
+      </c>
+      <c r="B2978" s="137"/>
+    </row>
+    <row r="2979" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2979" s="136">
+        <v>44186</v>
+      </c>
+      <c r="B2979" s="137">
+        <v>3.5834999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2731" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-22-2020 17-12-38
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="143" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E563F784-413D-493B-A73B-C6CA1A386172}"/>
+  <xr:revisionPtr revIDLastSave="144" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B1641724-E433-4921-8896-89457C0D0E8C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1301,13 +1301,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2979"/>
+  <dimension ref="A1:C2980"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B2968" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B2973" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A2979" sqref="A2979"/>
+      <selection pane="bottomRight" activeCell="A2980" sqref="A2980"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23633,6 +23633,14 @@
         <v>3.5834999999999999</v>
       </c>
     </row>
+    <row r="2980" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2980" s="136">
+        <v>44187</v>
+      </c>
+      <c r="B2980" s="137">
+        <v>3.6145999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2731" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-23-2020 17-05-28
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B1641724-E433-4921-8896-89457C0D0E8C}"/>
+  <xr:revisionPtr revIDLastSave="147" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{41E21E0A-2C14-4871-B51C-9556AE4A2947}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="ExportCuadro" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ExportCuadro!$A$3:$B$2731</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ExportCuadro!$A$3:$B$2981</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -1301,13 +1301,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2980"/>
+  <dimension ref="A1:C2981"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B2973" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B2978" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A2980" sqref="A2980"/>
+      <selection pane="bottomRight" activeCell="A2981" sqref="A2981"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23641,8 +23641,16 @@
         <v>3.6145999999999998</v>
       </c>
     </row>
+    <row r="2981" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2981" s="136">
+        <v>44188</v>
+      </c>
+      <c r="B2981" s="137">
+        <v>3.55</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A3:B2731" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A3:B2981" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-23-2020 21-02-48
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="147" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{41E21E0A-2C14-4871-B51C-9556AE4A2947}"/>
+  <xr:revisionPtr revIDLastSave="148" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F9B6D008-30E6-4188-82FF-2ABC0624234A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1301,13 +1301,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2981"/>
+  <dimension ref="A1:C2982"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B2978" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A2981" sqref="A2981"/>
+      <selection pane="bottomRight" activeCell="A2982" sqref="A2982"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23649,6 +23649,14 @@
         <v>3.55</v>
       </c>
     </row>
+    <row r="2982" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2982" s="136">
+        <v>44189</v>
+      </c>
+      <c r="B2982" s="137">
+        <v>3.5034000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2981" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-24-2020 20-52-05
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="148" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F9B6D008-30E6-4188-82FF-2ABC0624234A}"/>
+  <xr:revisionPtr revIDLastSave="149" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ABB591FB-E054-477D-9F29-C6FB9ED3EA30}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1301,13 +1301,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2982"/>
+  <dimension ref="A1:C2986"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B2978" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A2982" sqref="A2982"/>
+      <selection pane="bottomRight" activeCell="A2986" sqref="A2986"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23657,6 +23657,32 @@
         <v>3.5034000000000001</v>
       </c>
     </row>
+    <row r="2983" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2983" s="136">
+        <v>44190</v>
+      </c>
+      <c r="B2983" s="137"/>
+    </row>
+    <row r="2984" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2984" s="136">
+        <v>44191</v>
+      </c>
+      <c r="B2984" s="137"/>
+    </row>
+    <row r="2985" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2985" s="136">
+        <v>44192</v>
+      </c>
+      <c r="B2985" s="137"/>
+    </row>
+    <row r="2986" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2986" s="136">
+        <v>44193</v>
+      </c>
+      <c r="B2986" s="137">
+        <v>3.5503</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2981" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-29-2020 17-11-35
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="149" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ABB591FB-E054-477D-9F29-C6FB9ED3EA30}"/>
+  <xr:revisionPtr revIDLastSave="150" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{62CCFDBE-C25B-4C5C-94B8-2FFD5924D0FE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1301,13 +1301,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2986"/>
+  <dimension ref="A1:C2987"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B2978" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A2986" sqref="A2986"/>
+      <selection pane="bottomRight" activeCell="A2987" sqref="A2987"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23683,6 +23683,14 @@
         <v>3.5503</v>
       </c>
     </row>
+    <row r="2987" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2987" s="136">
+        <v>44194</v>
+      </c>
+      <c r="B2987" s="137">
+        <v>3.5247999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2981" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-30-2020 17-13-32
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="150" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{62CCFDBE-C25B-4C5C-94B8-2FFD5924D0FE}"/>
+  <xr:revisionPtr revIDLastSave="151" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0670D0E9-5C6B-409C-9F56-03A4B1E5D5B0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1301,13 +1301,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2987"/>
+  <dimension ref="A1:C2988"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B2978" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B2983" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A2987" sqref="A2987"/>
+      <selection pane="bottomRight" activeCell="B2988" sqref="B2988"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23691,6 +23691,14 @@
         <v>3.5247999999999999</v>
       </c>
     </row>
+    <row r="2988" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2988" s="136">
+        <v>44195</v>
+      </c>
+      <c r="B2988" s="137">
+        <v>3.5247999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2981" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-06-2021 16-30-52
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="159" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F47A8765-00C4-4D07-A718-85612A112A00}"/>
+  <xr:revisionPtr revIDLastSave="163" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A1469097-15DE-4BA6-B617-7A24BB094924}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -927,6 +927,18 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="40">
     <cellStyle name="20% - Énfasis1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1304,13 +1316,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2993"/>
+  <dimension ref="A1:C2995"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B2983" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B2988" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B2993" sqref="B2993"/>
+      <selection pane="bottomRight" activeCell="A2995" sqref="A2995"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23734,6 +23746,22 @@
         <v>3.5586000000000002</v>
       </c>
     </row>
+    <row r="2994" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2994" s="140">
+        <v>44201</v>
+      </c>
+      <c r="B2994" s="139">
+        <v>3.5148999999999999</v>
+      </c>
+    </row>
+    <row r="2995" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2995" s="142">
+        <v>44202</v>
+      </c>
+      <c r="B2995" s="141">
+        <v>3.5579999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2981" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-11-2021 15-26-25
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="163" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A1469097-15DE-4BA6-B617-7A24BB094924}"/>
+  <xr:revisionPtr revIDLastSave="168" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{28585B46-DBE3-4B42-AA80-16313C5D4861}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -939,6 +939,18 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="40">
     <cellStyle name="20% - Énfasis1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1316,13 +1328,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2995"/>
+  <dimension ref="A1:C3000"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B2988" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B2991" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A2995" sqref="A2995"/>
+      <selection pane="bottomRight" activeCell="A3000" sqref="A3000"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23762,6 +23774,42 @@
         <v>3.5579999999999998</v>
       </c>
     </row>
+    <row r="2996" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2996" s="144">
+        <v>44203</v>
+      </c>
+      <c r="B2996" s="143">
+        <v>3.6263000000000001</v>
+      </c>
+    </row>
+    <row r="2997" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2997" s="146">
+        <v>44204</v>
+      </c>
+      <c r="B2997" s="145">
+        <v>3.6425999999999998</v>
+      </c>
+    </row>
+    <row r="2998" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2998" s="146">
+        <v>44205</v>
+      </c>
+      <c r="B2998" s="145"/>
+    </row>
+    <row r="2999" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2999" s="146">
+        <v>44206</v>
+      </c>
+      <c r="B2999" s="145"/>
+    </row>
+    <row r="3000" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3000" s="146">
+        <v>44207</v>
+      </c>
+      <c r="B3000" s="145">
+        <v>3.7044999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2981" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-13-2021 17-07-16
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="168" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{28585B46-DBE3-4B42-AA80-16313C5D4861}"/>
+  <xr:revisionPtr revIDLastSave="172" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7ABD99CE-11CB-4EA4-A013-6C595C384E6E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -951,6 +951,18 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="40">
     <cellStyle name="20% - Énfasis1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1328,13 +1340,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3000"/>
+  <dimension ref="A1:C3002"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B2991" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B2996" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A3000" sqref="A3000"/>
+      <selection pane="bottomRight" activeCell="B3004" sqref="B3004"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23810,6 +23822,22 @@
         <v>3.7044999999999999</v>
       </c>
     </row>
+    <row r="3001" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3001" s="148">
+        <v>44208</v>
+      </c>
+      <c r="B3001" s="147">
+        <v>3.6823000000000001</v>
+      </c>
+    </row>
+    <row r="3002" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3002" s="150">
+        <v>44209</v>
+      </c>
+      <c r="B3002" s="149">
+        <v>3.5606</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2981" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-14-2021 17-05-40
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="172" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7ABD99CE-11CB-4EA4-A013-6C595C384E6E}"/>
+  <xr:revisionPtr revIDLastSave="174" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CD1B1E44-7FB4-4651-A2FE-36012A490215}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -963,6 +963,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="40">
     <cellStyle name="20% - Énfasis1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1340,13 +1346,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3002"/>
+  <dimension ref="A1:C3003"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B2996" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B3004" sqref="B3004"/>
+      <selection pane="bottomRight" activeCell="A3003" sqref="A3003"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23838,6 +23844,14 @@
         <v>3.5606</v>
       </c>
     </row>
+    <row r="3003" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3003" s="152">
+        <v>44210</v>
+      </c>
+      <c r="B3003" s="151">
+        <v>3.6126999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2981" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-15-2021 17-14-02
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="174" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CD1B1E44-7FB4-4651-A2FE-36012A490215}"/>
+  <xr:revisionPtr revIDLastSave="176" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{64203D73-711E-4928-BACA-C7FF624ADD20}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -969,6 +969,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="40">
     <cellStyle name="20% - Énfasis1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1346,13 +1352,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3003"/>
+  <dimension ref="A1:C3004"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B2996" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A3003" sqref="A3003"/>
+      <selection pane="bottomRight" activeCell="A3004" sqref="A3004"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23852,6 +23858,14 @@
         <v>3.6126999999999998</v>
       </c>
     </row>
+    <row r="3004" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3004" s="154">
+        <v>44211</v>
+      </c>
+      <c r="B3004" s="153">
+        <v>3.6263000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2981" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-16-2021 17-12-47
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="176" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{64203D73-711E-4928-BACA-C7FF624ADD20}"/>
+  <xr:revisionPtr revIDLastSave="179" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{378569ED-4D11-4446-BC59-CA71001086C5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1352,13 +1352,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3004"/>
+  <dimension ref="A1:C3008"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B2996" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B3005" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A3004" sqref="A3004"/>
+      <selection pane="bottomRight" activeCell="A3008" sqref="A3008"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23866,6 +23866,34 @@
         <v>3.6263000000000001</v>
       </c>
     </row>
+    <row r="3005" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3005" s="154">
+        <v>44211</v>
+      </c>
+      <c r="B3005" s="153">
+        <v>3.6263000000000001</v>
+      </c>
+    </row>
+    <row r="3006" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3006" s="154">
+        <v>44212</v>
+      </c>
+      <c r="B3006" s="153"/>
+    </row>
+    <row r="3007" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3007" s="154">
+        <v>44213</v>
+      </c>
+      <c r="B3007" s="153"/>
+    </row>
+    <row r="3008" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3008" s="154">
+        <v>44214</v>
+      </c>
+      <c r="B3008" s="153">
+        <v>3.6467000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2981" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-18-2021 20-57-02
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="179" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{378569ED-4D11-4446-BC59-CA71001086C5}"/>
+  <xr:revisionPtr revIDLastSave="181" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0D63E842-5AA8-4E1A-8BA4-56D80AF77635}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -975,6 +975,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="40">
     <cellStyle name="20% - Énfasis1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1352,13 +1358,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3008"/>
+  <dimension ref="A1:C3009"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B3005" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A3008" sqref="A3008"/>
+      <selection pane="bottomRight" activeCell="A3009" sqref="A3009"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23894,6 +23900,14 @@
         <v>3.6467000000000001</v>
       </c>
     </row>
+    <row r="3009" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3009" s="156">
+        <v>44215</v>
+      </c>
+      <c r="B3009" s="155">
+        <v>3.6004</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2981" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-20-2021 17-05-27
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="181" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0D63E842-5AA8-4E1A-8BA4-56D80AF77635}"/>
+  <xr:revisionPtr revIDLastSave="183" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BEE6736E-1206-4A1C-BCCC-CE5B5601D509}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -981,6 +981,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="40">
     <cellStyle name="20% - Énfasis1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1358,13 +1364,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3009"/>
+  <dimension ref="A1:C3010"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B3005" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A3009" sqref="A3009"/>
+      <selection pane="bottomRight" activeCell="A3010" sqref="A3010"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23908,6 +23914,14 @@
         <v>3.6004</v>
       </c>
     </row>
+    <row r="3010" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3010" s="158">
+        <v>44216</v>
+      </c>
+      <c r="B3010" s="157">
+        <v>3.6143000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2981" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-21-2021 17-08-15
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="183" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BEE6736E-1206-4A1C-BCCC-CE5B5601D509}"/>
+  <xr:revisionPtr revIDLastSave="185" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{64FE4BA1-4912-4633-96DA-7B9905039781}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -987,6 +987,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="40">
     <cellStyle name="20% - Énfasis1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1364,13 +1370,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3010"/>
+  <dimension ref="A1:C3011"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B3005" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A3010" sqref="A3010"/>
+      <selection pane="bottomRight" activeCell="A3011" sqref="A3011"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23922,6 +23928,14 @@
         <v>3.6143000000000001</v>
       </c>
     </row>
+    <row r="3011" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3011" s="160">
+        <v>44217</v>
+      </c>
+      <c r="B3011" s="159">
+        <v>3.6067</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2981" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-22-2021 17-05-51
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="185" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{64FE4BA1-4912-4633-96DA-7B9905039781}"/>
+  <xr:revisionPtr revIDLastSave="187" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A9E71FAB-97EC-4F08-9DD9-AD92F91C3297}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="161">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -993,6 +993,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="40">
     <cellStyle name="20% - Énfasis1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1370,13 +1376,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3011"/>
+  <dimension ref="A1:C3012"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B3005" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A3011" sqref="A3011"/>
+      <selection pane="bottomRight" activeCell="A3012" sqref="A3012"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23936,6 +23942,14 @@
         <v>3.6067</v>
       </c>
     </row>
+    <row r="3012" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3012" s="162">
+        <v>44218</v>
+      </c>
+      <c r="B3012" s="161">
+        <v>3.6469999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2981" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-23-2021 17-10-58
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="187" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A9E71FAB-97EC-4F08-9DD9-AD92F91C3297}"/>
+  <xr:revisionPtr revIDLastSave="188" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{80FC5DE2-D588-47B8-B84F-FA6C49836E8B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1376,13 +1376,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3012"/>
+  <dimension ref="A1:C3015"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B3005" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B3015" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A3012" sqref="A3012"/>
+      <selection pane="bottomRight" activeCell="A3015" sqref="A3015"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23950,6 +23950,26 @@
         <v>3.6469999999999998</v>
       </c>
     </row>
+    <row r="3013" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3013" s="162">
+        <v>44219</v>
+      </c>
+      <c r="B3013" s="161"/>
+    </row>
+    <row r="3014" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3014" s="162">
+        <v>44220</v>
+      </c>
+      <c r="B3014" s="161"/>
+    </row>
+    <row r="3015" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3015" s="162">
+        <v>44221</v>
+      </c>
+      <c r="B3015" s="161">
+        <v>3.6352000000000002</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2981" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-26-2021 17-13-48
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="188" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{80FC5DE2-D588-47B8-B84F-FA6C49836E8B}"/>
+  <xr:revisionPtr revIDLastSave="189" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5510B259-C518-4A98-A01C-03E740ED3854}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1376,13 +1376,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3015"/>
+  <dimension ref="A1:C3016"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B3015" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A3015" sqref="A3015"/>
+      <selection pane="bottomRight" activeCell="B3016" sqref="B3016"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23970,6 +23970,14 @@
         <v>3.6352000000000002</v>
       </c>
     </row>
+    <row r="3016" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3016" s="162">
+        <v>44222</v>
+      </c>
+      <c r="B3016" s="161">
+        <v>3.6257999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2981" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-27-2021 17-14-17
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="189" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5510B259-C518-4A98-A01C-03E740ED3854}"/>
+  <xr:revisionPtr revIDLastSave="191" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1BCB8B8E-2B3F-4D35-87DC-1BAE4E0A39A0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -999,6 +999,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="40">
     <cellStyle name="20% - Énfasis1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1376,13 +1382,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3016"/>
+  <dimension ref="A1:C3017"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B3015" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B3016" sqref="B3016"/>
+      <selection pane="bottomRight" activeCell="A3017" sqref="A3017"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23978,6 +23984,14 @@
         <v>3.6257999999999999</v>
       </c>
     </row>
+    <row r="3017" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3017" s="164">
+        <v>44223</v>
+      </c>
+      <c r="B3017" s="163">
+        <v>3.6131000000000002</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2981" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-28-2021 17-07-24
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="191" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1BCB8B8E-2B3F-4D35-87DC-1BAE4E0A39A0}"/>
+  <xr:revisionPtr revIDLastSave="192" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{577A3DF7-045B-4AB7-B933-31BCC14B47DF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1005,6 +1005,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="40">
     <cellStyle name="20% - Énfasis1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1382,13 +1388,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3017"/>
+  <dimension ref="A1:C3018"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B3015" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B3018" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A3017" sqref="A3017"/>
+      <selection pane="bottomRight" activeCell="A3018" sqref="A3018"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23992,6 +23998,14 @@
         <v>3.6131000000000002</v>
       </c>
     </row>
+    <row r="3018" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3018" s="165">
+        <v>44224</v>
+      </c>
+      <c r="B3018" s="166">
+        <v>3.6320999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2981" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-29-2021 17-11-25
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="192" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{577A3DF7-045B-4AB7-B933-31BCC14B47DF}"/>
+  <xr:revisionPtr revIDLastSave="194" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F0F82F49-31B9-4D8A-AC68-7ED71F2B59F8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1011,6 +1011,12 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="40">
     <cellStyle name="20% - Énfasis1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1388,13 +1394,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3018"/>
+  <dimension ref="A1:C3019"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B3018" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A3018" sqref="A3018"/>
+      <selection pane="bottomRight" activeCell="A3019" sqref="A3019"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24006,6 +24012,14 @@
         <v>3.6320999999999999</v>
       </c>
     </row>
+    <row r="3019" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3019" s="168">
+        <v>44225</v>
+      </c>
+      <c r="B3019" s="167">
+        <v>3.5476999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2981" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 04-21-2021 19-48-47
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="283" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E4C60C11-45BF-4BD0-8B34-95BDF59FD106}"/>
+  <xr:revisionPtr revIDLastSave="285" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9FB007EC-DDFF-4BBD-BF81-1F3B2F27F643}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1407,10 +1407,10 @@
   <dimension ref="A1:C3100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B3099" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B3100" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A3099" sqref="A3099"/>
+      <selection pane="bottomRight" activeCell="A3100" sqref="A3100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24683,8 +24683,12 @@
       </c>
     </row>
     <row r="3100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3100" s="11"/>
-      <c r="B3100" s="11"/>
+      <c r="A3100" s="167">
+        <v>44307</v>
+      </c>
+      <c r="B3100" s="168">
+        <v>4.2567000000000004</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A3:B2981" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 04-25-2021 17-12-03
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="289" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{168519D3-54CC-4202-BFED-4DBE687ABFC0}"/>
+  <xr:revisionPtr revIDLastSave="294" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{027D67D0-8A05-458D-8B0C-8F0D05A872EA}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="4">
   <si>
     <t>Dia</t>
   </si>
@@ -1404,13 +1404,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3102"/>
+  <dimension ref="A1:C3105"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B3102" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B3105" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A3102" sqref="A3102"/>
+      <selection pane="bottomRight" activeCell="A3105" sqref="A3105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24706,6 +24706,30 @@
         <v>4.2907999999999999</v>
       </c>
     </row>
+    <row r="3103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3103" s="167">
+        <v>44310</v>
+      </c>
+      <c r="B3103" s="168" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3104" s="167">
+        <v>44311</v>
+      </c>
+      <c r="B3104" s="168" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3105" s="167">
+        <v>44312</v>
+      </c>
+      <c r="B3105" s="168">
+        <v>4.2735000000000003</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B2981" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-01-2021 19-28-46
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/ID_SERIE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="306" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{80C30107-39D1-47CD-AC52-C2763D5625F8}"/>
+  <xr:revisionPtr revIDLastSave="308" documentId="114_{48AD900D-2E37-4D9E-A957-CB5E47DCDC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C56C4AB5-D4BE-48B8-99A7-15CFB3A40234}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="4">
   <si>
     <t>Dia</t>
   </si>
@@ -1404,13 +1404,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3109"/>
+  <dimension ref="A1:C3112"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B3108" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B3112" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A3109" sqref="A3109"/>
+      <selection pane="bottomRight" activeCell="A3112" sqref="A3112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24762,6 +24762,30 @@
         <v>4.4817</v>
       </c>
     </row>
+    <row r="3110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3110" s="167">
+        <v>44317</v>
+      </c>
+      <c r="B3110" s="168" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3111" s="167">
+        <v>44318</v>
+      </c>
+      <c r="B3111" s="168" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3112" s="167">
+        <v>44319</v>
+      </c>
+      <c r="B3112" s="168">
+        <v>4.4855999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:B3106" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>